<commit_message>
Ya no acepta numeros negativos
</commit_message>
<xml_diff>
--- a/Analisis del problema.xlsx
+++ b/Analisis del problema.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
@@ -10,17 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -30,7 +20,7 @@
     <author>ESTUDIANTE</author>
   </authors>
   <commentList>
-    <comment ref="N2" authorId="0">
+    <comment ref="Q3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0">
+    <comment ref="S3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P14" authorId="0">
+    <comment ref="S15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Comprención del Problema</t>
   </si>
@@ -147,7 +137,19 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Si aplicamos sustitución podemos reducir la cantidad de operacionesa una sola</t>
+    <t>Si aplicamos sustitución podemos reducir la cantidad de operaciones a una sola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenguaje </t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Metodo de ordenamiento</t>
+  </si>
+  <si>
+    <t>Insert</t>
   </si>
 </sst>
 </file>
@@ -306,6 +308,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,9 +318,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -331,14 +333,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -605,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -618,129 +612,130 @@
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="L1" s="2" t="s">
+    <row r="1" spans="1:21">
+      <c r="I1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="G2" s="1"/>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="G2" s="1"/>
-      <c r="L2" s="3">
+    <row r="3" spans="1:21">
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="O3" s="3">
         <v>0.05</v>
       </c>
-      <c r="M2" s="2">
+      <c r="P3" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
-        <f>+L2*$N$9/$L$9</f>
+      <c r="Q3" s="2">
+        <f t="shared" ref="Q3:Q9" si="0">+O3*$Q$10/$O$10</f>
         <v>3.5</v>
       </c>
-      <c r="O2" s="2">
-        <v>5</v>
-      </c>
-      <c r="P2" s="2">
-        <f>+O2*N2/10</f>
+      <c r="R3" s="2">
+        <v>5</v>
+      </c>
+      <c r="S3" s="2">
+        <f>+R3*Q3/10</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="B3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="L3" s="3">
+    <row r="4" spans="1:21">
+      <c r="O4" s="3">
         <v>0.15</v>
       </c>
-      <c r="M3" s="2">
+      <c r="P4" s="2">
         <v>2</v>
       </c>
-      <c r="N3" s="2">
-        <f>+L3*$N$9/$L$9</f>
+      <c r="Q4" s="2">
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
-      <c r="O3" s="2">
-        <v>10</v>
-      </c>
-      <c r="P3" s="2">
-        <f t="shared" ref="P3:P8" si="0">+O3*N3/10</f>
+      <c r="R4" s="2">
+        <v>10</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" ref="S4:S9" si="1">+R4*Q4/10</f>
         <v>10.5</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="L4" s="3">
+    <row r="5" spans="1:21">
+      <c r="A5" s="2"/>
+      <c r="B5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="O5" s="3">
         <v>0.05</v>
       </c>
-      <c r="M4" s="2">
+      <c r="P5" s="2">
         <v>3</v>
       </c>
-      <c r="N4" s="2">
-        <f t="shared" ref="N4:N8" si="1">+L4*$N$9/$L$9</f>
+      <c r="Q5" s="2">
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="O4" s="2">
+      <c r="R5" s="2">
         <v>4</v>
       </c>
-      <c r="P4" s="2">
-        <f t="shared" si="0"/>
+      <c r="S5" s="2">
+        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="2"/>
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-      <c r="L5" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="M5" s="2">
-        <v>4</v>
-      </c>
-      <c r="N5" s="2">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="O5" s="2">
-        <v>3</v>
-      </c>
-      <c r="P5" s="2">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -768,25 +763,25 @@
       <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="M6" s="2">
-        <v>5</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="O6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="P6" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="R6" s="2">
+        <v>3</v>
+      </c>
+      <c r="S6" s="2">
         <f t="shared" si="1"/>
-        <v>13.3</v>
-      </c>
-      <c r="O6" s="2">
-        <v>10</v>
-      </c>
-      <c r="P6" s="2">
-        <f>+O6*N6/10</f>
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -814,25 +809,25 @@
       <c r="I7" s="2">
         <v>70</v>
       </c>
-      <c r="L7" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="M7" s="2">
-        <v>6</v>
-      </c>
-      <c r="N7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="O7" s="2">
-        <v>5</v>
+      <c r="O7" s="3">
+        <v>0.19</v>
       </c>
       <c r="P7" s="2">
-        <f>+O7*N7/10</f>
-        <v>0.35000000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="0"/>
+        <v>13.3</v>
+      </c>
+      <c r="R7" s="2">
+        <v>10</v>
+      </c>
+      <c r="S7" s="2">
+        <f>+R7*Q7/10</f>
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="10">
         <v>2</v>
       </c>
@@ -860,25 +855,25 @@
       <c r="I8" s="2">
         <v>40.880000000000003</v>
       </c>
-      <c r="L8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="M8" s="2">
-        <v>7</v>
-      </c>
-      <c r="N8" s="2">
-        <f t="shared" si="1"/>
-        <v>10.5</v>
-      </c>
-      <c r="O8" s="2">
-        <v>8</v>
+      <c r="O8" s="3">
+        <v>0.01</v>
       </c>
       <c r="P8" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="2">
         <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="R8" s="2">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2">
+        <f>+R8*Q8/10</f>
+        <v>0.35000000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="10">
         <v>3</v>
       </c>
@@ -904,31 +899,28 @@
         <v>8</v>
       </c>
       <c r="I9" s="2">
-        <f>+P9</f>
+        <f>+S10</f>
         <v>44.1</v>
       </c>
-      <c r="L9" s="3">
-        <f>SUM(L2:L8)</f>
-        <v>1</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="2">
-        <v>70</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="5">
-        <f>SUM(P2:P8)</f>
-        <v>44.1</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="O9" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="P9" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+      <c r="R9" s="2">
+        <v>8</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="10">
         <v>4</v>
       </c>
@@ -956,12 +948,28 @@
       <c r="I10" s="2">
         <v>37.03</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="O10" s="3">
+        <f>SUM(O3:O9)</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>70</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="5">
+        <f>SUM(S3:S9)</f>
+        <v>44.1</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="10">
         <v>5</v>
       </c>
@@ -989,168 +997,175 @@
       <c r="I11" s="2">
         <v>26.39</v>
       </c>
-      <c r="L11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="B12" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="O11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="9"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="L13" s="2" t="s">
+      <c r="O12" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="O14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="R14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="S14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="L14" s="3">
+    <row r="15" spans="1:21">
+      <c r="O15" s="3">
         <v>0.05</v>
       </c>
-      <c r="M14" s="2">
+      <c r="P15" s="2">
         <v>1</v>
       </c>
-      <c r="O14" s="2">
-        <v>5</v>
-      </c>
-      <c r="P14" s="2">
-        <f>+(($M$21*L14/$L$21)*O14/10)</f>
+      <c r="R15" s="2">
+        <v>5</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" ref="S15:S21" si="2">+(($P$22*O15/$O$22)*R15/10)</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
-      <c r="L15" s="3">
+    <row r="16" spans="1:21">
+      <c r="O16" s="3">
         <v>0.15</v>
       </c>
-      <c r="M15" s="2">
+      <c r="P16" s="2">
         <v>2</v>
       </c>
-      <c r="O15" s="2">
+      <c r="R16" s="2">
         <v>6</v>
       </c>
-      <c r="P15" s="2">
-        <f t="shared" ref="P15:P20" si="2">+(($M$21*L15/$L$21)*O15/10)</f>
+      <c r="S16" s="2">
+        <f t="shared" si="2"/>
         <v>6.3</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="L16" s="3">
+    <row r="17" spans="15:20">
+      <c r="O17" s="3">
         <v>0.05</v>
       </c>
-      <c r="M16" s="2">
+      <c r="P17" s="2">
         <v>3</v>
       </c>
-      <c r="O16" s="2">
+      <c r="R17" s="2">
         <v>9</v>
       </c>
-      <c r="P16" s="2">
+      <c r="S17" s="2">
         <f t="shared" si="2"/>
         <v>3.15</v>
       </c>
     </row>
-    <row r="17" spans="12:17">
-      <c r="L17" s="3">
+    <row r="18" spans="15:20">
+      <c r="O18" s="3">
         <v>0.4</v>
       </c>
-      <c r="M17" s="2">
+      <c r="P18" s="2">
         <v>4</v>
       </c>
-      <c r="O17" s="2">
+      <c r="R18" s="2">
         <v>4</v>
       </c>
-      <c r="P17" s="2">
+      <c r="S18" s="2">
         <f t="shared" si="2"/>
         <v>11.2</v>
       </c>
     </row>
-    <row r="18" spans="12:17">
-      <c r="L18" s="3">
+    <row r="19" spans="15:20">
+      <c r="O19" s="3">
         <v>0.19</v>
       </c>
-      <c r="M18" s="2">
-        <v>5</v>
-      </c>
-      <c r="O18" s="2">
+      <c r="P19" s="2">
+        <v>5</v>
+      </c>
+      <c r="R19" s="2">
         <v>1</v>
       </c>
-      <c r="P18" s="2">
+      <c r="S19" s="2">
         <f t="shared" si="2"/>
         <v>1.33</v>
       </c>
     </row>
-    <row r="19" spans="12:17">
-      <c r="L19" s="3">
+    <row r="20" spans="15:20">
+      <c r="O20" s="3">
         <v>0.01</v>
       </c>
-      <c r="M19" s="2">
+      <c r="P20" s="2">
         <v>6</v>
       </c>
-      <c r="O19" s="2">
+      <c r="R20" s="2">
         <v>8</v>
       </c>
-      <c r="P19" s="2">
+      <c r="S20" s="2">
         <f t="shared" si="2"/>
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="20" spans="12:17">
-      <c r="L20" s="3">
+    <row r="21" spans="15:20">
+      <c r="O21" s="3">
         <v>0.15</v>
       </c>
-      <c r="M20" s="2">
+      <c r="P21" s="2">
         <v>7</v>
       </c>
-      <c r="O20" s="2">
+      <c r="R21" s="2">
         <v>2</v>
       </c>
-      <c r="P20" s="2">
+      <c r="S21" s="2">
         <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
     </row>
-    <row r="21" spans="12:17">
-      <c r="L21" s="3">
-        <f>SUM(L14:L20)</f>
+    <row r="22" spans="15:20">
+      <c r="O22" s="3">
+        <f>SUM(O15:O21)</f>
         <v>1</v>
       </c>
-      <c r="M21" s="5">
+      <c r="P22" s="5">
         <v>70</v>
       </c>
-      <c r="P21" s="2">
-        <f>SUM(P14:P20)</f>
+      <c r="S22" s="2">
+        <f>SUM(S15:S21)</f>
         <v>26.389999999999997</v>
       </c>
-      <c r="Q21" s="7" t="s">
+      <c r="T22" s="7" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="O12:U12"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B12:H12"/>
-    <mergeCell ref="L11:R11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>